<commit_message>
rebuilding site Mon 14 Sep 2020 08:16:14 PM EDT
</commit_message>
<xml_diff>
--- a/engineering/courses/mae101/docs/fatigue.xlsx
+++ b/engineering/courses/mae101/docs/fatigue.xlsx
@@ -29,6 +29,7 @@
         <sz val="13"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Fatigue Failure Data : T</t>
     </r>
@@ -39,6 +40,7 @@
         <sz val="13"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">he number of cycles required for the clips to break</t>
     </r>
@@ -77,6 +79,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -99,6 +102,7 @@
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -106,6 +110,7 @@
       <sz val="13"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -113,17 +118,20 @@
       <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -273,13 +281,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.13"/>
@@ -489,7 +497,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="n">
-        <v>3</v>
+        <v>7.5</v>
       </c>
       <c r="B33" s="4" t="n">
         <v>1</v>
@@ -497,7 +505,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="n">
-        <v>4</v>
+        <v>9.5</v>
       </c>
       <c r="B34" s="4" t="n">
         <v>1</v>
@@ -505,39 +513,39 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="n">
-        <v>4.5</v>
+        <v>10</v>
       </c>
       <c r="B35" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="n">
-        <v>5</v>
+        <v>10.5</v>
       </c>
       <c r="B36" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="n">
-        <v>5.5</v>
+        <v>11</v>
       </c>
       <c r="B37" s="4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="n">
-        <v>6</v>
+        <v>11.5</v>
       </c>
       <c r="B38" s="4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="n">
-        <v>7</v>
+        <v>12.5</v>
       </c>
       <c r="B39" s="4" t="n">
         <v>1</v>
@@ -545,7 +553,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="n">
-        <v>7.5</v>
+        <v>13</v>
       </c>
       <c r="B40" s="4" t="n">
         <v>1</v>
@@ -553,9 +561,17 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B41" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="B42" s="4" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>